<commit_message>
Updated documentation for CRDMA DVM test cases Updated application to change X axis label for the survey name reports (Page 1, 20)
</commit_message>
<xml_diff>
--- a/CRDMA/docs/test_cases/packages/CDVM/CRDMA CDVM Test Cases.xlsx
+++ b/CRDMA/docs/test_cases/packages/CDVM/CRDMA CDVM Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16725" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16725" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Category 1 DVM Tests" sheetId="5" r:id="rId1"/>
@@ -284,7 +284,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +303,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -317,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -340,6 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -996,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1013,7 @@
     <col min="2" max="2" width="47.5703125" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.42578125" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1031,7 +1038,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1051,7 +1058,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -1071,7 +1078,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1091,7 +1098,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B5" s="8" t="s">

</xml_diff>